<commit_message>
Update DateBase/orders/International Ever Green_2025-10-29.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/International Ever Green_2025-10-29.xlsx
+++ b/DateBase/orders/International Ever Green_2025-10-29.xlsx
@@ -612,6 +612,9 @@
       <c r="C21" t="str">
         <v>321_雪柳叶_Spiraea  leaves_undefined_1bunch</v>
       </c>
+      <c r="F21" t="str">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -673,7 +676,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>0242415828101211520554050205050100</v>
+        <v>0242415828101211520554050205050101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>